<commit_message>
Convert zeros to blanks where data is missing
</commit_message>
<xml_diff>
--- a/tests/fixtures/preprocessing_input_output.xlsx
+++ b/tests/fixtures/preprocessing_input_output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfrank1\Git\wattile\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDE5617-2248-45A4-9576-B4706812843C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEFEEB7-012E-481F-9726-13BDD635BA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="38700" windowHeight="15435" activeTab="3" xr2:uid="{F1F4070D-BE47-474C-891B-1069753761B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Source Data" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="39">
   <si>
     <t>ts</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Closed: Right</t>
+  </si>
+  <si>
+    <t>var2_max</t>
   </si>
 </sst>
 </file>
@@ -557,25 +560,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -595,7 +593,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -610,7 +608,7 @@
       <c r="H2" s="11"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -620,7 +618,7 @@
       <c r="F3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -630,7 +628,7 @@
       <c r="F4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -640,7 +638,7 @@
       <c r="F5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -650,7 +648,7 @@
       <c r="F6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -660,7 +658,7 @@
       <c r="F7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -670,7 +668,7 @@
       <c r="F8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -680,7 +678,7 @@
       <c r="F9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -690,7 +688,7 @@
       <c r="F10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -704,7 +702,7 @@
       <c r="F11" s="7"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -714,7 +712,7 @@
       <c r="F12" s="8"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -724,7 +722,7 @@
       <c r="F13" s="8"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -734,7 +732,7 @@
       <c r="F14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -744,7 +742,7 @@
       <c r="F15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -754,7 +752,7 @@
       <c r="F16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -764,7 +762,7 @@
       <c r="F17" s="8"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -778,7 +776,7 @@
       <c r="F18" s="5"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -788,7 +786,7 @@
       <c r="F19" s="9"/>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
@@ -798,7 +796,7 @@
       <c r="F20" s="9"/>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -808,7 +806,7 @@
       <c r="F21" s="9"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -818,7 +816,7 @@
       <c r="F22" s="9"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -828,7 +826,7 @@
       <c r="F23" s="9"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -838,7 +836,7 @@
       <c r="F24" s="9"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -848,7 +846,7 @@
       <c r="F25" s="9"/>
       <c r="H25" s="9"/>
     </row>
-    <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -872,21 +870,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5D4585-C138-4964-808C-23662B4256BE}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:N1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -900,7 +893,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -913,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -930,7 +923,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -947,7 +940,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -973,21 +966,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9064E003-B4DE-442C-8517-9A6F7D126DD6}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:M1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>IF(ISBLANK('Source Data'!A1),"",'Source Data'!A1)</f>
         <v>ts</v>
@@ -1005,7 +993,7 @@
         <v>target</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f>IF(ISBLANK('Source Data'!A2),"",'Source Data'!A2)</f>
         <v>2022-07-12 07:00:00+06:00</v>
@@ -1023,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A3),"",'Source Data'!A3)</f>
         <v>2022-07-12 07:01:00+06:00</v>
@@ -1041,7 +1029,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A4),"",'Source Data'!A4)</f>
         <v>2022-07-12 07:01:53+06:00</v>
@@ -1059,7 +1047,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A5),"",'Source Data'!A5)</f>
         <v>2022-07-12 07:02:00+06:00</v>
@@ -1077,7 +1065,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A6),"",'Source Data'!A6)</f>
         <v>2022-07-12 07:03:00+06:00</v>
@@ -1095,7 +1083,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A7),"",'Source Data'!A7)</f>
         <v>2022-07-12 07:03:17+06:00</v>
@@ -1113,7 +1101,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A8),"",'Source Data'!A8)</f>
         <v>2022-07-12 07:04:00+06:00</v>
@@ -1131,7 +1119,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A9),"",'Source Data'!A9)</f>
         <v>2022-07-12 07:04:02+06:00</v>
@@ -1149,7 +1137,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A10),"",'Source Data'!A10)</f>
         <v>2022-07-12 07:04:59+06:00</v>
@@ -1167,7 +1155,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="str">
         <f>IF(ISBLANK('Source Data'!A11),"",'Source Data'!A11)</f>
         <v>2022-07-12 07:05:00+06:00</v>
@@ -1185,7 +1173,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A12),"",'Source Data'!A12)</f>
         <v>2022-07-12 07:06:00+06:00</v>
@@ -1203,7 +1191,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A13),"",'Source Data'!A13)</f>
         <v>2022-07-12 07:06:22+06:00</v>
@@ -1221,7 +1209,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A14),"",'Source Data'!A14)</f>
         <v>2022-07-12 07:07:00+06:00</v>
@@ -1239,7 +1227,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A15),"",'Source Data'!A15)</f>
         <v>2022-07-12 07:08:00+06:00</v>
@@ -1257,7 +1245,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A16),"",'Source Data'!A16)</f>
         <v>2022-07-12 07:09:00+06:00</v>
@@ -1275,7 +1263,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A17),"",'Source Data'!A17)</f>
         <v>2022-07-12 07:09:46+06:00</v>
@@ -1293,7 +1281,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
         <f>IF(ISBLANK('Source Data'!A18),"",'Source Data'!A18)</f>
         <v>2022-07-12 07:10:00+06:00</v>
@@ -1311,7 +1299,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A19),"",'Source Data'!A19)</f>
         <v>2022-07-12 07:11:00+06:00</v>
@@ -1329,7 +1317,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A20),"",'Source Data'!A20)</f>
         <v>2022-07-12 07:11:17+06:00</v>
@@ -1347,7 +1335,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A21),"",'Source Data'!A21)</f>
         <v>2022-07-12 07:12:00+06:00</v>
@@ -1365,7 +1353,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A22),"",'Source Data'!A22)</f>
         <v>2022-07-12 07:13:00+06:00</v>
@@ -1383,7 +1371,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A23),"",'Source Data'!A23)</f>
         <v>2022-07-12 07:13:34+06:00</v>
@@ -1401,7 +1389,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A24),"",'Source Data'!A24)</f>
         <v>2022-07-12 07:14:00+06:00</v>
@@ -1419,7 +1407,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="str">
         <f>IF(ISBLANK('Source Data'!A25),"",'Source Data'!A25)</f>
         <v>2022-07-12 07:14:26+06:00</v>
@@ -1437,7 +1425,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="str">
         <f>IF(ISBLANK('Source Data'!A26),"",'Source Data'!A26)</f>
         <v>2022-07-12 07:15:00+06:00</v>
@@ -1466,25 +1454,20 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P1" sqref="I1:P1048576"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1492,150 +1475,150 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
       </c>
       <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <f>IFERROR(MIN('Source Data'!$B2:$B10),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B10),MIN('Source Data'!$B2:$B10),""),"")</f>
         <v>0</v>
       </c>
       <c r="C2">
-        <f>IFERROR(AVERAGE('Source Data'!$B2:$B10),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C10),MIN('Source Data'!$C2:$C10),""),"")</f>
+        <v>0.2</v>
+      </c>
+      <c r="D2">
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B10),MAX('Source Data'!$B2:$B10),""),"")</f>
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C10),MAX('Source Data'!$C2:$C10),""),"")</f>
+        <v>5.9</v>
+      </c>
+      <c r="F2">
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B10),AVERAGE('Source Data'!$B2:$B10),""),"")</f>
         <v>2</v>
       </c>
-      <c r="D2">
-        <f>IFERROR(MAX('Source Data'!$B2:$B10),"")</f>
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <f>IFERROR(MIN('Source Data'!$C2:$C10),"")</f>
-        <v>0.2</v>
-      </c>
-      <c r="F2">
-        <f>IFERROR(AVERAGE('Source Data'!$C2:$C10),"")</f>
+      <c r="G2">
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C10),AVERAGE('Source Data'!$C2:$C10),""),"")</f>
         <v>3.2750000000000004</v>
-      </c>
-      <c r="G2">
-        <f>IFERROR(MAX('Source Data'!$C2:$C10),"")</f>
-        <v>5.9</v>
       </c>
       <c r="H2">
         <f>'Source Data'!$D2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <f>IFERROR(MIN('Source Data'!$B11:$B17),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B11:$B17),MIN('Source Data'!$B11:$B17),""),"")</f>
         <v>5</v>
       </c>
       <c r="C3">
-        <f>IFERROR(AVERAGE('Source Data'!$B11:$B17),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C11:$C17),MIN('Source Data'!$C11:$C17),""),"")</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D3">
+        <f>IFERROR(IF(COUNT('Source Data'!$B11:$B17),MAX('Source Data'!$B11:$B17),""),"")</f>
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <f>IFERROR(IF(COUNT('Source Data'!$C11:$C17),MAX('Source Data'!$C11:$C17),""),"")</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F3">
+        <f>IFERROR(IF(COUNT('Source Data'!$B11:$B17),AVERAGE('Source Data'!$B11:$B17),""),"")</f>
         <v>7</v>
       </c>
-      <c r="D3">
-        <f>IFERROR(MAX('Source Data'!$B11:$B17),"")</f>
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <f>IFERROR(MIN('Source Data'!$C11:$C17),"")</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F3">
-        <f>IFERROR(AVERAGE('Source Data'!$C11:$C17),"")</f>
+      <c r="G3">
+        <f>IFERROR(IF(COUNT('Source Data'!$C11:$C17),AVERAGE('Source Data'!$C11:$C17),""),"")</f>
         <v>3.4</v>
-      </c>
-      <c r="G3">
-        <f>IFERROR(MAX('Source Data'!$C11:$C17),"")</f>
-        <v>4.5999999999999996</v>
       </c>
       <c r="H3">
         <f>'Source Data'!D$11</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4">
-        <f>IFERROR(MIN('Source Data'!$B18:$B25),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B18:$B25),MIN('Source Data'!$B18:$B25),""),"")</f>
         <v>10</v>
       </c>
       <c r="C4">
-        <f>IFERROR(AVERAGE('Source Data'!$B18:$B25),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C18:$C25),MIN('Source Data'!$C18:$C25),""),"")</f>
+        <v>1.7</v>
+      </c>
+      <c r="D4">
+        <f>IFERROR(IF(COUNT('Source Data'!$B18:$B25),MAX('Source Data'!$B18:$B25),""),"")</f>
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <f>IFERROR(IF(COUNT('Source Data'!$C18:$C25),MAX('Source Data'!$C18:$C25),""),"")</f>
+        <v>3.4</v>
+      </c>
+      <c r="F4">
+        <f>IFERROR(IF(COUNT('Source Data'!$B18:$B25),AVERAGE('Source Data'!$B18:$B25),""),"")</f>
         <v>12</v>
       </c>
-      <c r="D4">
-        <f>IFERROR(MAX('Source Data'!$B18:$B25),"")</f>
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <f>IFERROR(MIN('Source Data'!$C18:$C25),"")</f>
-        <v>1.7</v>
-      </c>
-      <c r="F4">
-        <f>IFERROR(AVERAGE('Source Data'!$C18:$C25),"")</f>
+      <c r="G4">
+        <f>IFERROR(IF(COUNT('Source Data'!$C18:$C25),AVERAGE('Source Data'!$C18:$C25),""),"")</f>
         <v>2.5666666666666664</v>
-      </c>
-      <c r="G4">
-        <f>IFERROR(MAX('Source Data'!$C18:$C25),"")</f>
-        <v>3.4</v>
       </c>
       <c r="H4">
         <f>'Source Data'!D$18</f>
         <v>-0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5">
-        <f>IFERROR(MIN('Source Data'!$B26:$B26),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B26:$B26),MIN('Source Data'!$B26:$B26),""),"")</f>
         <v>15</v>
       </c>
-      <c r="C5">
-        <f>IFERROR(AVERAGE('Source Data'!$B26:$B26),"")</f>
+      <c r="C5" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C26:$C26),MIN('Source Data'!$C26:$C26),""),"")</f>
+        <v/>
+      </c>
+      <c r="D5">
+        <f>IFERROR(IF(COUNT('Source Data'!$B26:$B26),MAX('Source Data'!$B26:$B26),""),"")</f>
         <v>15</v>
       </c>
-      <c r="D5">
-        <f>IFERROR(MAX('Source Data'!$B26:$B26),"")</f>
+      <c r="E5" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C26:$C26),MAX('Source Data'!$C26:$C26),""),"")</f>
+        <v/>
+      </c>
+      <c r="F5">
+        <f>IFERROR(IF(COUNT('Source Data'!$B26:$B26),AVERAGE('Source Data'!$B26:$B26),""),"")</f>
         <v>15</v>
       </c>
-      <c r="E5">
-        <f>IFERROR(MIN('Source Data'!$C26:$C26),"")</f>
-        <v>0</v>
-      </c>
-      <c r="F5" t="str">
-        <f>IFERROR(AVERAGE('Source Data'!$C26:$C26),"")</f>
-        <v/>
-      </c>
-      <c r="G5">
-        <f>IFERROR(MAX('Source Data'!$C26:$C26),"")</f>
-        <v>0</v>
+      <c r="G5" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C26:$C26),AVERAGE('Source Data'!$C26:$C26),""),"")</f>
+        <v/>
       </c>
       <c r="H5">
         <f>'Source Data'!D$26</f>
@@ -1651,26 +1634,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1A6B31-9A64-4D26-B4EA-A15592EC69C5}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1:O1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1678,150 +1654,150 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
       </c>
       <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2">
-        <f>IFERROR(MIN('Source Data'!$B2:$B10),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B10),MIN('Source Data'!$B2:$B10),""),"")</f>
         <v>0</v>
       </c>
       <c r="C2">
-        <f>IFERROR(AVERAGE('Source Data'!$B2:$B10),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C10),MIN('Source Data'!$C2:$C10),""),"")</f>
+        <v>0.2</v>
+      </c>
+      <c r="D2">
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B10),MAX('Source Data'!$B2:$B10),""),"")</f>
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C10),MAX('Source Data'!$C2:$C10),""),"")</f>
+        <v>5.9</v>
+      </c>
+      <c r="F2">
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B10),AVERAGE('Source Data'!$B2:$B10),""),"")</f>
         <v>2</v>
       </c>
-      <c r="D2">
-        <f>IFERROR(MAX('Source Data'!$B2:$B10),"")</f>
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <f>IFERROR(MIN('Source Data'!$C2:$C10),"")</f>
-        <v>0.2</v>
-      </c>
-      <c r="F2">
-        <f>IFERROR(AVERAGE('Source Data'!$C2:$C10),"")</f>
+      <c r="G2">
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C10),AVERAGE('Source Data'!$C2:$C10),""),"")</f>
         <v>3.2750000000000004</v>
-      </c>
-      <c r="G2">
-        <f>IFERROR(MAX('Source Data'!$C2:$C10),"")</f>
-        <v>5.9</v>
       </c>
       <c r="H2">
         <f>'Source Data'!$D2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <f>IFERROR(MIN('Source Data'!$B11:$B17),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B11:$B17),MIN('Source Data'!$B11:$B17),""),"")</f>
         <v>5</v>
       </c>
       <c r="C3">
-        <f>IFERROR(AVERAGE('Source Data'!$B11:$B17),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C11:$C17),MIN('Source Data'!$C11:$C17),""),"")</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D3">
+        <f>IFERROR(IF(COUNT('Source Data'!$B11:$B17),MAX('Source Data'!$B11:$B17),""),"")</f>
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <f>IFERROR(IF(COUNT('Source Data'!$C11:$C17),MAX('Source Data'!$C11:$C17),""),"")</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F3">
+        <f>IFERROR(IF(COUNT('Source Data'!$B11:$B17),AVERAGE('Source Data'!$B11:$B17),""),"")</f>
         <v>7</v>
       </c>
-      <c r="D3">
-        <f>IFERROR(MAX('Source Data'!$B11:$B17),"")</f>
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <f>IFERROR(MIN('Source Data'!$C11:$C17),"")</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F3">
-        <f>IFERROR(AVERAGE('Source Data'!$C11:$C17),"")</f>
+      <c r="G3">
+        <f>IFERROR(IF(COUNT('Source Data'!$C11:$C17),AVERAGE('Source Data'!$C11:$C17),""),"")</f>
         <v>3.4</v>
-      </c>
-      <c r="G3">
-        <f>IFERROR(MAX('Source Data'!$C11:$C17),"")</f>
-        <v>4.5999999999999996</v>
       </c>
       <c r="H3">
         <f>'Source Data'!D$11</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4">
-        <f>IFERROR(MIN('Source Data'!$B18:$B25),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B18:$B25),MIN('Source Data'!$B18:$B25),""),"")</f>
         <v>10</v>
       </c>
       <c r="C4">
-        <f>IFERROR(AVERAGE('Source Data'!$B18:$B25),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C18:$C25),MIN('Source Data'!$C18:$C25),""),"")</f>
+        <v>1.7</v>
+      </c>
+      <c r="D4">
+        <f>IFERROR(IF(COUNT('Source Data'!$B18:$B25),MAX('Source Data'!$B18:$B25),""),"")</f>
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <f>IFERROR(IF(COUNT('Source Data'!$C18:$C25),MAX('Source Data'!$C18:$C25),""),"")</f>
+        <v>3.4</v>
+      </c>
+      <c r="F4">
+        <f>IFERROR(IF(COUNT('Source Data'!$B18:$B25),AVERAGE('Source Data'!$B18:$B25),""),"")</f>
         <v>12</v>
       </c>
-      <c r="D4">
-        <f>IFERROR(MAX('Source Data'!$B18:$B25),"")</f>
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <f>IFERROR(MIN('Source Data'!$C18:$C25),"")</f>
-        <v>1.7</v>
-      </c>
-      <c r="F4">
-        <f>IFERROR(AVERAGE('Source Data'!$C18:$C25),"")</f>
+      <c r="G4">
+        <f>IFERROR(IF(COUNT('Source Data'!$C18:$C25),AVERAGE('Source Data'!$C18:$C25),""),"")</f>
         <v>2.5666666666666664</v>
-      </c>
-      <c r="G4">
-        <f>IFERROR(MAX('Source Data'!$C18:$C25),"")</f>
-        <v>3.4</v>
       </c>
       <c r="H4">
         <f>'Source Data'!D$18</f>
         <v>-0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B5">
-        <f>IFERROR(MIN('Source Data'!$B26:$B26),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B26:$B26),MIN('Source Data'!$B26:$B26),""),"")</f>
         <v>15</v>
       </c>
-      <c r="C5">
-        <f>IFERROR(AVERAGE('Source Data'!$B26:$B26),"")</f>
+      <c r="C5" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C26:$C26),MIN('Source Data'!$C26:$C26),""),"")</f>
+        <v/>
+      </c>
+      <c r="D5">
+        <f>IFERROR(IF(COUNT('Source Data'!$B26:$B26),MAX('Source Data'!$B26:$B26),""),"")</f>
         <v>15</v>
       </c>
-      <c r="D5">
-        <f>IFERROR(MAX('Source Data'!$B26:$B26),"")</f>
+      <c r="E5" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C26:$C26),MAX('Source Data'!$C26:$C26),""),"")</f>
+        <v/>
+      </c>
+      <c r="F5">
+        <f>IFERROR(IF(COUNT('Source Data'!$B26:$B26),AVERAGE('Source Data'!$B26:$B26),""),"")</f>
         <v>15</v>
       </c>
-      <c r="E5">
-        <f>IFERROR(MIN('Source Data'!$C26:$C26),"")</f>
-        <v>0</v>
-      </c>
-      <c r="F5" t="str">
-        <f>IFERROR(AVERAGE('Source Data'!$C26:$C26),"")</f>
-        <v/>
-      </c>
-      <c r="G5">
-        <f>IFERROR(MAX('Source Data'!$C26:$C26),"")</f>
-        <v>0</v>
+      <c r="G5" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C26:$C26),AVERAGE('Source Data'!$C26:$C26),""),"")</f>
+        <v/>
       </c>
       <c r="H5">
         <f>'Source Data'!D$26</f>
@@ -1837,26 +1813,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC848CF-F235-4F44-90BD-EF805546C846}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1:Q1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1864,150 +1833,150 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
       </c>
       <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B2">
-        <f>IFERROR(MIN('Source Data'!$B2:$B2),"")</f>
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <f>IFERROR(AVERAGE('Source Data'!$B2:$B2),"")</f>
-        <v>0</v>
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B2),MIN('Source Data'!$B2:$B2),""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C2),MIN('Source Data'!$C2:$C2),""),"")</f>
+        <v/>
       </c>
       <c r="D2">
-        <f>IFERROR(MAX('Source Data'!$B2:$B2),"")</f>
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f>IFERROR(MIN('Source Data'!$C2:$C2),"")</f>
-        <v>0</v>
-      </c>
-      <c r="F2" t="str">
-        <f>IFERROR(AVERAGE('Source Data'!$C2:$C2),"")</f>
-        <v/>
-      </c>
-      <c r="G2">
-        <f>IFERROR(MAX('Source Data'!$C2:$C2),"")</f>
-        <v>0</v>
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B2),MAX('Source Data'!$B2:$B2),""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C2),MAX('Source Data'!$C2:$C2),""),"")</f>
+        <v/>
+      </c>
+      <c r="F2">
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B2),AVERAGE('Source Data'!$B2:$B2),""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C2),AVERAGE('Source Data'!$C2:$C2),""),"")</f>
+        <v/>
       </c>
       <c r="H2">
         <f>'Source Data'!$D2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <f>IFERROR(MIN('Source Data'!$B3:$B11),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B3:$B11),MIN('Source Data'!$B3:$B11),""),"")</f>
         <v>1</v>
       </c>
       <c r="C3">
-        <f>IFERROR(AVERAGE('Source Data'!$B3:$B11),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C3:$C11),MIN('Source Data'!$C3:$C11),""),"")</f>
+        <v>0.2</v>
+      </c>
+      <c r="D3">
+        <f>IFERROR(IF(COUNT('Source Data'!$B3:$B11),MAX('Source Data'!$B3:$B11),""),"")</f>
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <f>IFERROR(IF(COUNT('Source Data'!$C3:$C11),MAX('Source Data'!$C3:$C11),""),"")</f>
+        <v>5.9</v>
+      </c>
+      <c r="F3">
+        <f>IFERROR(IF(COUNT('Source Data'!$B3:$B11),AVERAGE('Source Data'!$B3:$B11),""),"")</f>
         <v>3</v>
       </c>
-      <c r="D3">
-        <f>IFERROR(MAX('Source Data'!$B3:$B11),"")</f>
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <f>IFERROR(MIN('Source Data'!$C3:$C11),"")</f>
-        <v>0.2</v>
-      </c>
-      <c r="F3">
-        <f>IFERROR(AVERAGE('Source Data'!$C3:$C11),"")</f>
+      <c r="G3">
+        <f>IFERROR(IF(COUNT('Source Data'!$C3:$C11),AVERAGE('Source Data'!$C3:$C11),""),"")</f>
         <v>3.2750000000000004</v>
-      </c>
-      <c r="G3">
-        <f>IFERROR(MAX('Source Data'!$C3:$C11),"")</f>
-        <v>5.9</v>
       </c>
       <c r="H3">
         <f>'Source Data'!D$11</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <f>IFERROR(MIN('Source Data'!$B12:$B18),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B12:$B18),MIN('Source Data'!$B12:$B18),""),"")</f>
         <v>6</v>
       </c>
       <c r="C4">
-        <f>IFERROR(AVERAGE('Source Data'!$B12:$B18),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C12:$C18),MIN('Source Data'!$C12:$C18),""),"")</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D4">
+        <f>IFERROR(IF(COUNT('Source Data'!$B12:$B18),MAX('Source Data'!$B12:$B18),""),"")</f>
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <f>IFERROR(IF(COUNT('Source Data'!$C12:$C18),MAX('Source Data'!$C12:$C18),""),"")</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F4">
+        <f>IFERROR(IF(COUNT('Source Data'!$B12:$B18),AVERAGE('Source Data'!$B12:$B18),""),"")</f>
         <v>8</v>
       </c>
-      <c r="D4">
-        <f>IFERROR(MAX('Source Data'!$B12:$B18),"")</f>
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <f>IFERROR(MIN('Source Data'!$C12:$C18),"")</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F4">
-        <f>IFERROR(AVERAGE('Source Data'!$C12:$C18),"")</f>
+      <c r="G4">
+        <f>IFERROR(IF(COUNT('Source Data'!$C12:$C18),AVERAGE('Source Data'!$C12:$C18),""),"")</f>
         <v>3.4</v>
-      </c>
-      <c r="G4">
-        <f>IFERROR(MAX('Source Data'!$C12:$C18),"")</f>
-        <v>4.5999999999999996</v>
       </c>
       <c r="H4">
         <f>'Source Data'!D$18</f>
         <v>-0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5">
-        <f>IFERROR(MIN('Source Data'!$B19:$B26),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B19:$B26),MIN('Source Data'!$B19:$B26),""),"")</f>
         <v>11</v>
       </c>
       <c r="C5">
-        <f>IFERROR(AVERAGE('Source Data'!$B19:$B26),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C19:$C26),MIN('Source Data'!$C19:$C26),""),"")</f>
+        <v>1.7</v>
+      </c>
+      <c r="D5">
+        <f>IFERROR(IF(COUNT('Source Data'!$B19:$B26),MAX('Source Data'!$B19:$B26),""),"")</f>
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <f>IFERROR(IF(COUNT('Source Data'!$C19:$C26),MAX('Source Data'!$C19:$C26),""),"")</f>
+        <v>3.4</v>
+      </c>
+      <c r="F5">
+        <f>IFERROR(IF(COUNT('Source Data'!$B19:$B26),AVERAGE('Source Data'!$B19:$B26),""),"")</f>
         <v>13</v>
       </c>
-      <c r="D5">
-        <f>IFERROR(MAX('Source Data'!$B19:$B26),"")</f>
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <f>IFERROR(MIN('Source Data'!$C19:$C26),"")</f>
-        <v>1.7</v>
-      </c>
-      <c r="F5">
-        <f>IFERROR(AVERAGE('Source Data'!$C19:$C26),"")</f>
+      <c r="G5">
+        <f>IFERROR(IF(COUNT('Source Data'!$C19:$C26),AVERAGE('Source Data'!$C19:$C26),""),"")</f>
         <v>2.5666666666666664</v>
-      </c>
-      <c r="G5">
-        <f>IFERROR(MAX('Source Data'!$C19:$C26),"")</f>
-        <v>3.4</v>
       </c>
       <c r="H5">
         <f>'Source Data'!D$26</f>
@@ -2023,26 +1992,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74039D4-57E2-4B2E-892C-22528E3D2DD5}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1:Q1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2050,150 +2012,150 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
       </c>
       <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <f>IFERROR(MIN('Source Data'!$B2:$B2),"")</f>
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <f>IFERROR(AVERAGE('Source Data'!$B2:$B2),"")</f>
-        <v>0</v>
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B2),MIN('Source Data'!$B2:$B2),""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C2),MIN('Source Data'!$C2:$C2),""),"")</f>
+        <v/>
       </c>
       <c r="D2">
-        <f>IFERROR(MAX('Source Data'!$B2:$B2),"")</f>
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f>IFERROR(MIN('Source Data'!$C2:$C2),"")</f>
-        <v>0</v>
-      </c>
-      <c r="F2" t="str">
-        <f>IFERROR(AVERAGE('Source Data'!$C2:$C2),"")</f>
-        <v/>
-      </c>
-      <c r="G2">
-        <f>IFERROR(MAX('Source Data'!$C2:$C2),"")</f>
-        <v>0</v>
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B2),MAX('Source Data'!$B2:$B2),""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C2),MAX('Source Data'!$C2:$C2),""),"")</f>
+        <v/>
+      </c>
+      <c r="F2">
+        <f>IFERROR(IF(COUNT('Source Data'!$B2:$B2),AVERAGE('Source Data'!$B2:$B2),""),"")</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IFERROR(IF(COUNT('Source Data'!$C2:$C2),AVERAGE('Source Data'!$C2:$C2),""),"")</f>
+        <v/>
       </c>
       <c r="H2">
         <f>'Source Data'!$D2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <f>IFERROR(MIN('Source Data'!$B3:$B11),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B3:$B11),MIN('Source Data'!$B3:$B11),""),"")</f>
         <v>1</v>
       </c>
       <c r="C3">
-        <f>IFERROR(AVERAGE('Source Data'!$B3:$B11),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C3:$C11),MIN('Source Data'!$C3:$C11),""),"")</f>
+        <v>0.2</v>
+      </c>
+      <c r="D3">
+        <f>IFERROR(IF(COUNT('Source Data'!$B3:$B11),MAX('Source Data'!$B3:$B11),""),"")</f>
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <f>IFERROR(IF(COUNT('Source Data'!$C3:$C11),MAX('Source Data'!$C3:$C11),""),"")</f>
+        <v>5.9</v>
+      </c>
+      <c r="F3">
+        <f>IFERROR(IF(COUNT('Source Data'!$B3:$B11),AVERAGE('Source Data'!$B3:$B11),""),"")</f>
         <v>3</v>
       </c>
-      <c r="D3">
-        <f>IFERROR(MAX('Source Data'!$B3:$B11),"")</f>
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <f>IFERROR(MIN('Source Data'!$C3:$C11),"")</f>
-        <v>0.2</v>
-      </c>
-      <c r="F3">
-        <f>IFERROR(AVERAGE('Source Data'!$C3:$C11),"")</f>
+      <c r="G3">
+        <f>IFERROR(IF(COUNT('Source Data'!$C3:$C11),AVERAGE('Source Data'!$C3:$C11),""),"")</f>
         <v>3.2750000000000004</v>
-      </c>
-      <c r="G3">
-        <f>IFERROR(MAX('Source Data'!$C3:$C11),"")</f>
-        <v>5.9</v>
       </c>
       <c r="H3">
         <f>'Source Data'!D$11</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4">
-        <f>IFERROR(MIN('Source Data'!$B12:$B18),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B12:$B18),MIN('Source Data'!$B12:$B18),""),"")</f>
         <v>6</v>
       </c>
       <c r="C4">
-        <f>IFERROR(AVERAGE('Source Data'!$B12:$B18),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C12:$C18),MIN('Source Data'!$C12:$C18),""),"")</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D4">
+        <f>IFERROR(IF(COUNT('Source Data'!$B12:$B18),MAX('Source Data'!$B12:$B18),""),"")</f>
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <f>IFERROR(IF(COUNT('Source Data'!$C12:$C18),MAX('Source Data'!$C12:$C18),""),"")</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F4">
+        <f>IFERROR(IF(COUNT('Source Data'!$B12:$B18),AVERAGE('Source Data'!$B12:$B18),""),"")</f>
         <v>8</v>
       </c>
-      <c r="D4">
-        <f>IFERROR(MAX('Source Data'!$B12:$B18),"")</f>
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <f>IFERROR(MIN('Source Data'!$C12:$C18),"")</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F4">
-        <f>IFERROR(AVERAGE('Source Data'!$C12:$C18),"")</f>
+      <c r="G4">
+        <f>IFERROR(IF(COUNT('Source Data'!$C12:$C18),AVERAGE('Source Data'!$C12:$C18),""),"")</f>
         <v>3.4</v>
-      </c>
-      <c r="G4">
-        <f>IFERROR(MAX('Source Data'!$C12:$C18),"")</f>
-        <v>4.5999999999999996</v>
       </c>
       <c r="H4">
         <f>'Source Data'!D$18</f>
         <v>-0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5">
-        <f>IFERROR(MIN('Source Data'!$B19:$B26),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$B19:$B26),MIN('Source Data'!$B19:$B26),""),"")</f>
         <v>11</v>
       </c>
       <c r="C5">
-        <f>IFERROR(AVERAGE('Source Data'!$B19:$B26),"")</f>
+        <f>IFERROR(IF(COUNT('Source Data'!$C19:$C26),MIN('Source Data'!$C19:$C26),""),"")</f>
+        <v>1.7</v>
+      </c>
+      <c r="D5">
+        <f>IFERROR(IF(COUNT('Source Data'!$B19:$B26),MAX('Source Data'!$B19:$B26),""),"")</f>
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <f>IFERROR(IF(COUNT('Source Data'!$C19:$C26),MAX('Source Data'!$C19:$C26),""),"")</f>
+        <v>3.4</v>
+      </c>
+      <c r="F5">
+        <f>IFERROR(IF(COUNT('Source Data'!$B19:$B26),AVERAGE('Source Data'!$B19:$B26),""),"")</f>
         <v>13</v>
       </c>
-      <c r="D5">
-        <f>IFERROR(MAX('Source Data'!$B19:$B26),"")</f>
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <f>IFERROR(MIN('Source Data'!$C19:$C26),"")</f>
-        <v>1.7</v>
-      </c>
-      <c r="F5">
-        <f>IFERROR(AVERAGE('Source Data'!$C19:$C26),"")</f>
+      <c r="G5">
+        <f>IFERROR(IF(COUNT('Source Data'!$C19:$C26),AVERAGE('Source Data'!$C19:$C26),""),"")</f>
         <v>2.5666666666666664</v>
-      </c>
-      <c r="G5">
-        <f>IFERROR(MAX('Source Data'!$C19:$C26),"")</f>
-        <v>3.4</v>
       </c>
       <c r="H5">
         <f>'Source Data'!D$26</f>
@@ -2209,21 +2171,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E83A5D9-74C7-403F-9DAB-75EEC8CEDEB8}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:M1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2237,7 +2194,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2254,7 +2211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2271,7 +2228,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -2288,7 +2245,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -2310,21 +2267,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BCABCF5-2BAB-4B40-8E7D-3D1A91326744}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:K1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2338,7 +2290,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2355,7 +2307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2372,7 +2324,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2389,7 +2341,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
@@ -2411,21 +2363,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DF908F-770A-4C8B-8DB8-4F8CBCDCEC93}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:N1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2439,7 +2386,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -2452,7 +2399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2469,7 +2416,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2486,7 +2433,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>